<commit_message>
Fishbase comparison, annotated figures, addition data
Code created for comparison of data to fishbase log10a vs b. Figures for both fishbase comparison and including additional annotation included. Figures ending in 2 are the annotated graphs, which include fitted line, Rsquared (WIP), 95% confidence interval, and min and max lengths (approximate) for each species. Figures ending in log10a_b are the fishbase comparisons of reported a and b values. Additional data for both Spratelloides species collected in an attempt to better represent all lengths (additional data still needed).
</commit_message>
<xml_diff>
--- a/Albatross_Raw_Data/Calculated_variables.xlsx
+++ b/Albatross_Raw_Data/Calculated_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabes\Documents\AlbatrossPhillipinesLWR\Albatross_Raw_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708CDE42-00C0-4526-994E-9120F72655B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0905B6CD-FAE4-481A-B8B2-742A6AAEC992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -185,9 +185,6 @@
     <t>250_ft_seine</t>
   </si>
   <si>
-    <t>Ambassis_interruptus</t>
-  </si>
-  <si>
     <t>Palawan_stream_near_Chase_Head_village</t>
   </si>
   <si>
@@ -246,13 +243,16 @@
   </si>
   <si>
     <t>Max_TL</t>
+  </si>
+  <si>
+    <t>Ambassis_interrupta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +309,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -330,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -339,6 +345,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,13 +628,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
@@ -656,22 +668,22 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>9</v>
@@ -1132,7 +1144,7 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="3" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B15" s="3">
         <v>6</v>
@@ -1174,10 +1186,10 @@
         <v>8.17</v>
       </c>
       <c r="P15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q15" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>16</v>
@@ -1197,10 +1209,10 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="P16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q16" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>16</v>
@@ -1209,7 +1221,7 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -1251,10 +1263,10 @@
         <v>11.97</v>
       </c>
       <c r="P17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q17" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>16</v>
@@ -1265,7 +1277,7 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -1273,44 +1285,44 @@
       <c r="C18" s="3">
         <v>138978</v>
       </c>
-      <c r="D18">
-        <v>1.0985999999999999E-2</v>
-      </c>
-      <c r="E18" s="3">
-        <v>3.202E-3</v>
-      </c>
-      <c r="F18" s="3">
-        <v>2.9270740000000002</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0.18882599999999999</v>
+      <c r="D18" s="8">
+        <v>7.9120000000000006E-3</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1.284E-3</v>
+      </c>
+      <c r="F18" s="8">
+        <v>3.1549749999999999</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.10331</v>
       </c>
       <c r="I18" s="3">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="J18" s="3">
-        <v>0.21099999999999999</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="K18" s="3">
-        <v>1.6459999999999999</v>
+        <v>1.87</v>
       </c>
       <c r="L18" s="3">
-        <v>1</v>
+        <v>1.76</v>
       </c>
       <c r="M18" s="3">
-        <v>5.47</v>
+        <v>5.52</v>
       </c>
       <c r="N18" s="3">
-        <v>3.29</v>
+        <v>1.89</v>
       </c>
       <c r="O18" s="3">
         <v>6.35</v>
       </c>
       <c r="P18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q18" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="R18" s="4" t="s">
         <v>16</v>
@@ -1330,7 +1342,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="P19" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q19" s="3" t="s">
         <v>41</v>
@@ -1340,56 +1352,71 @@
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="3" t="s">
+      <c r="B20" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="B21" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="3">
+        <v>9</v>
+      </c>
+      <c r="C22" s="3">
+        <v>138930</v>
+      </c>
+      <c r="D22" s="8">
+        <v>5.9858000000000003E-3</v>
+      </c>
+      <c r="E22" s="8">
+        <v>7.4660000000000004E-4</v>
+      </c>
+      <c r="F22" s="8">
+        <v>3.1470501999999998</v>
+      </c>
+      <c r="G22" s="8">
+        <v>7.2609999999999994E-2</v>
+      </c>
+      <c r="I22" s="3">
+        <v>68</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="K22" s="3">
+        <v>1.7490000000000001</v>
+      </c>
+      <c r="L22" s="3">
+        <v>2.31</v>
+      </c>
+      <c r="M22" s="3">
+        <v>6.03</v>
+      </c>
+      <c r="N22" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="O22" s="3">
+        <v>6.73</v>
+      </c>
+      <c r="P22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="3">
+      <c r="Q22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="B23" s="7">
         <v>9</v>
-      </c>
-      <c r="C20" s="3">
-        <v>138930</v>
-      </c>
-      <c r="D20">
-        <v>5.3080000000000002E-3</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1.3489999999999999E-3</v>
-      </c>
-      <c r="F20" s="3">
-        <v>3.2163379999999999</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0.14682700000000001</v>
-      </c>
-      <c r="I20" s="3">
-        <v>42</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="K20" s="3">
-        <v>1.7490000000000001</v>
-      </c>
-      <c r="L20" s="3">
-        <v>3.25</v>
-      </c>
-      <c r="M20" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="N20" s="3">
-        <v>3.52</v>
-      </c>
-      <c r="O20" s="3">
-        <v>6.73</v>
-      </c>
-      <c r="P20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="R20" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added additional species and adjusted commands
Added D. duodecimalis, H, temminckii, and T. fucata, with all 3 figures included (except for H. temmickii bc it has no reported LWR). Added install.packages to commands pages for first time setup.
</commit_message>
<xml_diff>
--- a/Albatross_Raw_Data/Calculated_variables.xlsx
+++ b/Albatross_Raw_Data/Calculated_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabes\Documents\AlbatrossPhillipinesLWR\Albatross_Raw_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF4584B-BB77-426D-9073-E8D582572411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7330203-FEEE-492B-977C-F1225E16B91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="0" windowWidth="17580" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="121">
   <si>
     <t>Species</t>
   </si>
@@ -321,6 +321,84 @@
   </si>
   <si>
     <t>same</t>
+  </si>
+  <si>
+    <t>Hypoatherina_temminckii</t>
+  </si>
+  <si>
+    <t>Ticao_Island_San_Miguel_Harbor</t>
+  </si>
+  <si>
+    <t>21_Apr_08</t>
+  </si>
+  <si>
+    <t>Port_Busan_Busuanga_Island</t>
+  </si>
+  <si>
+    <t>17_Dec_08</t>
+  </si>
+  <si>
+    <t>unkown</t>
+  </si>
+  <si>
+    <t>Bolinao_Bay_Luzon</t>
+  </si>
+  <si>
+    <t>10_May_09</t>
+  </si>
+  <si>
+    <t>Busin_Harbor_Burias_Island</t>
+  </si>
+  <si>
+    <t>22_Apr_08</t>
+  </si>
+  <si>
+    <t>Atulayan_Bay_Luzon_Island</t>
+  </si>
+  <si>
+    <t>17_Jun_09</t>
+  </si>
+  <si>
+    <t>Parang_Mindanao</t>
+  </si>
+  <si>
+    <t>23_May_08</t>
+  </si>
+  <si>
+    <t>Taeniamia_fucata</t>
+  </si>
+  <si>
+    <t>W_Coast_of_Palawan_Endeavor_Strait</t>
+  </si>
+  <si>
+    <t>23_Dec_08</t>
+  </si>
+  <si>
+    <t>Dynamite</t>
+  </si>
+  <si>
+    <t>Rita_Island_Palawan</t>
+  </si>
+  <si>
+    <t>29_Dec_08</t>
+  </si>
+  <si>
+    <t>Linacapan_Island_Malcochin_Harbor</t>
+  </si>
+  <si>
+    <t>18_Dec_08</t>
+  </si>
+  <si>
+    <t>11 total</t>
+  </si>
+  <si>
+    <t>48 total</t>
+  </si>
+  <si>
+    <t>125 total</t>
+  </si>
+  <si>
+    <t>Doboatherina_duodecimalis</t>
   </si>
 </sst>
 </file>
@@ -391,7 +469,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,6 +488,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -423,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -439,6 +523,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2058,6 +2147,9 @@
       <c r="Q31" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="R31" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" s="3" t="s">
@@ -2096,6 +2188,9 @@
       <c r="Q32" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="R32" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="33" spans="1:18" s="8" customFormat="1">
       <c r="A33" s="9" t="s">
@@ -2222,6 +2317,9 @@
       <c r="Q35" s="3" t="s">
         <v>73</v>
       </c>
+      <c r="R35" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="36" spans="1:18" s="8" customFormat="1">
       <c r="A36" s="9" t="s">
@@ -2268,6 +2366,512 @@
       </c>
       <c r="O36" s="9">
         <v>67.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="7">
+        <v>10</v>
+      </c>
+      <c r="C37" s="3">
+        <v>136752</v>
+      </c>
+      <c r="I37" s="3">
+        <v>23</v>
+      </c>
+      <c r="J37">
+        <v>1.288</v>
+      </c>
+      <c r="K37">
+        <v>7.2430000000000003</v>
+      </c>
+      <c r="L37">
+        <v>52</v>
+      </c>
+      <c r="M37">
+        <v>93.7</v>
+      </c>
+      <c r="N37">
+        <v>58</v>
+      </c>
+      <c r="O37">
+        <v>103.7</v>
+      </c>
+      <c r="P37" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="R37" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="7">
+        <v>10</v>
+      </c>
+      <c r="C38" s="3">
+        <v>136726</v>
+      </c>
+      <c r="I38" s="3">
+        <v>25</v>
+      </c>
+      <c r="J38">
+        <v>0.442</v>
+      </c>
+      <c r="K38">
+        <v>7.1440000000000001</v>
+      </c>
+      <c r="L38">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="M38">
+        <v>72.2</v>
+      </c>
+      <c r="N38">
+        <v>39.9</v>
+      </c>
+      <c r="O38">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="P38" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="R38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" s="15" customFormat="1">
+      <c r="A39" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="14">
+        <v>10</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="J39" s="15">
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="K39" s="15">
+        <v>7.2430000000000003</v>
+      </c>
+      <c r="L39" s="15">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="M39" s="15">
+        <v>93.7</v>
+      </c>
+      <c r="N39" s="15">
+        <v>39.9</v>
+      </c>
+      <c r="O39" s="15">
+        <v>103.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="7">
+        <v>11</v>
+      </c>
+      <c r="C40" s="3">
+        <v>149423</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>2.548</v>
+      </c>
+      <c r="K40" t="s">
+        <v>94</v>
+      </c>
+      <c r="L40">
+        <v>50.2</v>
+      </c>
+      <c r="M40" t="s">
+        <v>94</v>
+      </c>
+      <c r="N40">
+        <v>62</v>
+      </c>
+      <c r="O40" t="s">
+        <v>94</v>
+      </c>
+      <c r="P40" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="R40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="7">
+        <v>11</v>
+      </c>
+      <c r="C41" s="3">
+        <v>149427</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="K41">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="L41">
+        <v>30.9</v>
+      </c>
+      <c r="M41">
+        <v>35</v>
+      </c>
+      <c r="N41">
+        <v>39.5</v>
+      </c>
+      <c r="O41">
+        <v>44.3</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="R41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="7">
+        <v>11</v>
+      </c>
+      <c r="C42" s="3">
+        <v>149429</v>
+      </c>
+      <c r="I42">
+        <v>8</v>
+      </c>
+      <c r="J42">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="K42">
+        <v>0.224</v>
+      </c>
+      <c r="L42">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="M42">
+        <v>23</v>
+      </c>
+      <c r="N42">
+        <v>21.7</v>
+      </c>
+      <c r="O42">
+        <v>27.8</v>
+      </c>
+      <c r="P42" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="R42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" s="15" customFormat="1">
+      <c r="A43" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" s="15">
+        <v>11</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="J43" s="15">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="K43" s="15">
+        <v>2.548</v>
+      </c>
+      <c r="L43" s="15">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="M43" s="15">
+        <v>50.2</v>
+      </c>
+      <c r="N43" s="15">
+        <v>21.7</v>
+      </c>
+      <c r="O43" s="15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" s="7">
+        <v>12</v>
+      </c>
+      <c r="C44" s="3">
+        <v>136831</v>
+      </c>
+      <c r="I44">
+        <v>37</v>
+      </c>
+      <c r="J44">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K44">
+        <v>2.4649999999999999</v>
+      </c>
+      <c r="L44">
+        <v>23</v>
+      </c>
+      <c r="M44">
+        <v>54.4</v>
+      </c>
+      <c r="N44">
+        <v>25.9</v>
+      </c>
+      <c r="O44">
+        <v>64.5</v>
+      </c>
+      <c r="P44" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q44" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="R44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" s="17" customFormat="1">
+      <c r="A45" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="16">
+        <v>12</v>
+      </c>
+      <c r="C45" s="12">
+        <v>136846</v>
+      </c>
+      <c r="I45" s="17">
+        <v>4</v>
+      </c>
+      <c r="J45" s="17">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="K45" s="17">
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="L45" s="17">
+        <v>43.8</v>
+      </c>
+      <c r="M45" s="17">
+        <v>49.1</v>
+      </c>
+      <c r="N45" s="17">
+        <v>51</v>
+      </c>
+      <c r="O45" s="17">
+        <v>58.3</v>
+      </c>
+      <c r="P45" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q45" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="R45" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" s="7">
+        <v>12</v>
+      </c>
+      <c r="C46" s="3">
+        <v>136827</v>
+      </c>
+      <c r="I46">
+        <v>6</v>
+      </c>
+      <c r="J46">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="K46">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="L46">
+        <v>22.9</v>
+      </c>
+      <c r="M46">
+        <v>45</v>
+      </c>
+      <c r="N46">
+        <v>24.9</v>
+      </c>
+      <c r="O46">
+        <v>52.2</v>
+      </c>
+      <c r="P46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q46" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" s="7">
+        <v>12</v>
+      </c>
+      <c r="C47" s="3">
+        <v>136851</v>
+      </c>
+      <c r="I47">
+        <v>17</v>
+      </c>
+      <c r="J47">
+        <v>0.376</v>
+      </c>
+      <c r="K47">
+        <v>1.9319999999999999</v>
+      </c>
+      <c r="L47">
+        <v>30.4</v>
+      </c>
+      <c r="M47">
+        <v>51</v>
+      </c>
+      <c r="N47">
+        <v>37.1</v>
+      </c>
+      <c r="O47">
+        <v>60.1</v>
+      </c>
+      <c r="P47" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>102</v>
+      </c>
+      <c r="R47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="7">
+        <v>12</v>
+      </c>
+      <c r="C48" s="3">
+        <v>136813</v>
+      </c>
+      <c r="I48">
+        <v>61</v>
+      </c>
+      <c r="J48">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="K48">
+        <v>4.6710000000000003</v>
+      </c>
+      <c r="L48">
+        <v>39.4</v>
+      </c>
+      <c r="M48">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="N48">
+        <v>44.7</v>
+      </c>
+      <c r="O48">
+        <v>83.6</v>
+      </c>
+      <c r="P48" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="R48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" s="15" customFormat="1">
+      <c r="A49" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" s="14">
+        <v>12</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I49" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="J49" s="15">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K49" s="15">
+        <v>4.6710000000000003</v>
+      </c>
+      <c r="L49" s="15">
+        <v>22.9</v>
+      </c>
+      <c r="M49" s="15">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="N49" s="15">
+        <v>24.9</v>
+      </c>
+      <c r="O49" s="15">
+        <v>83.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>